<commit_message>
Create £BANK (quick look)
</commit_message>
<xml_diff>
--- a/Case Studies/Quantum Bubble.xlsx
+++ b/Case Studies/Quantum Bubble.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\Case Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A82CD7-65A7-486C-BC14-667F7C002A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725D41AD-0204-4F44-A700-F74E916B44D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E04D14C-A4FC-48EC-9D0E-04E94F336D4D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>$IONQ</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Oct/Nov 24</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Upside Catalysts</t>
   </si>
   <si>
@@ -142,6 +139,21 @@
   </si>
   <si>
     <t>Potential benefits to medicine, finance &amp; crypto</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>R&amp;D of Quantum Computers</t>
+  </si>
+  <si>
+    <t>R&amp;D of Quantum Computers. Air Force Contract &amp; AWS Forte</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>NO REAL QUANTUM OPERATIONS - JUST NAME</t>
   </si>
 </sst>
 </file>
@@ -644,7 +656,7 @@
   <dimension ref="B2:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -671,12 +683,12 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="R2" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
       <c r="W2" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X2" s="12"/>
       <c r="Y2" s="12"/>
@@ -699,10 +711,10 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="R3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.2">
@@ -747,10 +759,10 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="R5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.2">
@@ -773,10 +785,10 @@
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="4"/>
@@ -789,12 +801,12 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="W7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="4"/>
@@ -1049,8 +1061,8 @@
       <c r="I28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N28" s="2" t="s">
-        <v>25</v>
+      <c r="L28" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.2">
@@ -1067,6 +1079,9 @@
         <f>H29*G29</f>
         <v>1074645</v>
       </c>
+      <c r="L29" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F30" s="1" t="s">
@@ -1082,6 +1097,9 @@
         <f t="shared" ref="I30:I33" si="0">H30*G30</f>
         <v>206441.5</v>
       </c>
+      <c r="L30" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F31" s="1" t="s">
@@ -1097,6 +1115,9 @@
         <f t="shared" si="0"/>
         <v>6534</v>
       </c>
+      <c r="L31" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="32" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F32" s="1" t="s">
@@ -1112,8 +1133,11 @@
         <f>H32*G32</f>
         <v>4777.3599999999997</v>
       </c>
-    </row>
-    <row r="33" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="L32" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F33" s="1" t="s">
         <v>1</v>
       </c>
@@ -1127,10 +1151,13 @@
         <f t="shared" si="0"/>
         <v>2811.2</v>
       </c>
-    </row>
-    <row r="34" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="L33" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F34" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G34" s="1">
         <v>6.1</v>
@@ -1143,7 +1170,7 @@
         <v>1372.5</v>
       </c>
     </row>
-    <row r="35" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F35" s="1" t="s">
         <v>8</v>
       </c>
@@ -1156,6 +1183,9 @@
       <c r="I35" s="10">
         <f>H35*G35</f>
         <v>1278.3900000000001</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>